<commit_message>
Homelessness NPA widget and uploader.
</commit_message>
<xml_diff>
--- a/dashboard_loader/housing_homelessness_npa_uploader/housing_homelessness_npa_data.xlsx
+++ b/dashboard_loader/housing_homelessness_npa_uploader/housing_homelessness_npa_data.xlsx
@@ -9,7 +9,7 @@
   </bookViews>
   <sheets>
     <sheet name="Data" sheetId="1" state="visible" r:id="rId2"/>
-    <sheet name="Sheet2" sheetId="2" state="visible" r:id="rId3"/>
+    <sheet name="Description" sheetId="2" state="visible" r:id="rId3"/>
   </sheets>
   <calcPr iterateCount="100" refMode="A1" iterate="false" iterateDelta="0.001"/>
   <extLst>
@@ -21,7 +21,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="37" uniqueCount="18">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="39" uniqueCount="20">
   <si>
     <r>
       <rPr>
@@ -89,6 +89,12 @@
     <t xml:space="preserve">Updated</t>
   </si>
   <si>
+    <t xml:space="preserve">Status</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Improving</t>
+  </si>
+  <si>
     <t xml:space="preserve">Desc Body</t>
   </si>
   <si>
@@ -117,32 +123,27 @@
   <numFmts count="1">
     <numFmt numFmtId="164" formatCode="General"/>
   </numFmts>
-  <fonts count="8">
-    <font>
-      <sz val="10"/>
-      <name val="Arial"/>
-      <family val="2"/>
-    </font>
-    <font>
-      <sz val="10"/>
-      <name val="Arial"/>
-      <family val="0"/>
-    </font>
-    <font>
-      <sz val="10"/>
-      <name val="Arial"/>
-      <family val="0"/>
-    </font>
-    <font>
-      <sz val="10"/>
-      <name val="Arial"/>
-      <family val="0"/>
-    </font>
+  <fonts count="7">
     <font>
       <sz val="10"/>
       <name val="Arial"/>
       <family val="2"/>
       <charset val="1"/>
+    </font>
+    <font>
+      <sz val="10"/>
+      <name val="Arial"/>
+      <family val="0"/>
+    </font>
+    <font>
+      <sz val="10"/>
+      <name val="Arial"/>
+      <family val="0"/>
+    </font>
+    <font>
+      <sz val="10"/>
+      <name val="Arial"/>
+      <family val="0"/>
     </font>
     <font>
       <b val="true"/>
@@ -210,17 +211,17 @@
     <xf numFmtId="44" fontId="1" fillId="0" borderId="0" applyFont="true" applyBorder="false" applyAlignment="false" applyProtection="false"/>
     <xf numFmtId="42" fontId="1" fillId="0" borderId="0" applyFont="true" applyBorder="false" applyAlignment="false" applyProtection="false"/>
     <xf numFmtId="9" fontId="1" fillId="0" borderId="0" applyFont="true" applyBorder="false" applyAlignment="false" applyProtection="false"/>
-    <xf numFmtId="164" fontId="4" fillId="0" borderId="0" applyFont="true" applyBorder="true" applyAlignment="true" applyProtection="true">
+    <xf numFmtId="164" fontId="0" fillId="0" borderId="0" applyFont="true" applyBorder="true" applyAlignment="true" applyProtection="true">
       <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
     </xf>
   </cellStyleXfs>
-  <cellXfs count="6">
+  <cellXfs count="5">
     <xf numFmtId="164" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="false" applyBorder="false" applyAlignment="false" applyProtection="false">
       <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
     </xf>
-    <xf numFmtId="164" fontId="5" fillId="0" borderId="0" xfId="0" applyFont="true" applyBorder="true" applyAlignment="true" applyProtection="false">
+    <xf numFmtId="164" fontId="4" fillId="0" borderId="0" xfId="0" applyFont="true" applyBorder="true" applyAlignment="true" applyProtection="false">
       <alignment horizontal="left" vertical="bottom" textRotation="0" wrapText="true" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
     </xf>
@@ -228,12 +229,8 @@
       <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
     </xf>
-    <xf numFmtId="164" fontId="7" fillId="0" borderId="0" xfId="20" applyFont="true" applyBorder="true" applyAlignment="true" applyProtection="false">
+    <xf numFmtId="164" fontId="6" fillId="0" borderId="0" xfId="20" applyFont="true" applyBorder="true" applyAlignment="true" applyProtection="false">
       <alignment horizontal="left" vertical="center" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
-      <protection locked="true" hidden="false"/>
-    </xf>
-    <xf numFmtId="164" fontId="4" fillId="0" borderId="0" xfId="0" applyFont="true" applyBorder="false" applyAlignment="true" applyProtection="false">
-      <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="true" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
     </xf>
     <xf numFmtId="164" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="true" applyBorder="false" applyAlignment="true" applyProtection="false">
@@ -248,7 +245,7 @@
     <cellStyle name="Currency" xfId="17" builtinId="4" customBuiltin="false"/>
     <cellStyle name="Currency [0]" xfId="18" builtinId="7" customBuiltin="false"/>
     <cellStyle name="Percent" xfId="19" builtinId="5" customBuiltin="false"/>
-    <cellStyle name="Normal_AIHW RoGS indicator concordance_NHA PI 13 4 yo health check" xfId="20" builtinId="53" customBuiltin="true"/>
+    <cellStyle name="Excel Built-in Explanatory Text" xfId="20" builtinId="53" customBuiltin="true"/>
   </cellStyles>
 </styleSheet>
 </file>
@@ -260,15 +257,19 @@
   </sheetPr>
   <dimension ref="A1:I18"/>
   <sheetViews>
-    <sheetView windowProtection="false" showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="false" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
-      <selection pane="topLeft" activeCell="B20" activeCellId="0" sqref="B20"/>
+    <sheetView windowProtection="true" showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="false" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
+      <pane xSplit="1" ySplit="19" topLeftCell="B20" activePane="bottomRight" state="frozen"/>
+      <selection pane="topLeft" activeCell="A1" activeCellId="0" sqref="A1"/>
+      <selection pane="topRight" activeCell="B1" activeCellId="0" sqref="B1"/>
+      <selection pane="bottomLeft" activeCell="A20" activeCellId="0" sqref="A20"/>
+      <selection pane="bottomRight" activeCell="D3" activeCellId="0" sqref="D3"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="12.8"/>
   <cols>
-    <col collapsed="false" hidden="false" max="1" min="1" style="0" width="11.5204081632653"/>
-    <col collapsed="false" hidden="false" max="2" min="2" style="0" width="57.0102040816327"/>
-    <col collapsed="false" hidden="false" max="1025" min="3" style="0" width="11.5204081632653"/>
+    <col collapsed="false" hidden="false" max="1" min="1" style="0" width="11.3418367346939"/>
+    <col collapsed="false" hidden="false" max="2" min="2" style="0" width="56.2908163265306"/>
+    <col collapsed="false" hidden="false" max="1025" min="3" style="0" width="11.3418367346939"/>
   </cols>
   <sheetData>
     <row r="1" customFormat="false" ht="59.95" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
@@ -455,17 +456,17 @@
   <sheetPr filterMode="false">
     <pageSetUpPr fitToPage="false"/>
   </sheetPr>
-  <dimension ref="A1:B6"/>
+  <dimension ref="A1:B7"/>
   <sheetViews>
     <sheetView windowProtection="false" showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="true" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
-      <selection pane="topLeft" activeCell="E6" activeCellId="0" sqref="E6"/>
+      <selection pane="topLeft" activeCell="B2" activeCellId="0" sqref="B2"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="12.8"/>
   <cols>
-    <col collapsed="false" hidden="false" max="1" min="1" style="0" width="10.4591836734694"/>
-    <col collapsed="false" hidden="false" max="2" min="2" style="0" width="59.6020408163265"/>
-    <col collapsed="false" hidden="false" max="1025" min="3" style="0" width="11.5204081632653"/>
+    <col collapsed="false" hidden="false" max="1" min="1" style="0" width="10.2602040816327"/>
+    <col collapsed="false" hidden="false" max="2" min="2" style="0" width="58.8571428571429"/>
+    <col collapsed="false" hidden="false" max="1025" min="3" style="0" width="11.3418367346939"/>
   </cols>
   <sheetData>
     <row r="1" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -476,42 +477,50 @@
         <v>2015</v>
       </c>
     </row>
-    <row r="2" customFormat="false" ht="68.95" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="2" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A2" s="2" t="s">
         <v>11</v>
       </c>
-      <c r="B2" s="4" t="s">
+      <c r="B2" s="2" t="s">
         <v>12</v>
       </c>
     </row>
     <row r="3" customFormat="false" ht="68.95" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A3" s="2" t="s">
+        <v>13</v>
+      </c>
       <c r="B3" s="4" t="s">
-        <v>13</v>
-      </c>
-    </row>
-    <row r="4" customFormat="false" ht="35.2" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+        <v>14</v>
+      </c>
+    </row>
+    <row r="4" customFormat="false" ht="68.95" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="B4" s="4" t="s">
-        <v>14</v>
-      </c>
-    </row>
-    <row r="5" customFormat="false" ht="35.95" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
-      <c r="A5" s="2" t="s">
         <v>15</v>
       </c>
+    </row>
+    <row r="5" customFormat="false" ht="35.2" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="B5" s="4" t="s">
         <v>16</v>
       </c>
     </row>
-    <row r="6" customFormat="false" ht="35.2" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A6" s="2"/>
-      <c r="B6" s="5" t="s">
+    <row r="6" customFormat="false" ht="35.95" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
+      <c r="A6" s="2" t="s">
         <v>17</v>
+      </c>
+      <c r="B6" s="4" t="s">
+        <v>18</v>
+      </c>
+    </row>
+    <row r="7" customFormat="false" ht="35.2" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A7" s="2"/>
+      <c r="B7" s="4" t="s">
+        <v>19</v>
       </c>
     </row>
   </sheetData>
   <printOptions headings="false" gridLines="false" gridLinesSet="true" horizontalCentered="false" verticalCentered="false"/>
   <pageMargins left="0.7875" right="0.7875" top="1.05277777777778" bottom="1.05277777777778" header="0.7875" footer="0.7875"/>
-  <pageSetup paperSize="9" scale="100" firstPageNumber="1" fitToWidth="1" fitToHeight="1" pageOrder="downThenOver" orientation="portrait" usePrinterDefaults="false" blackAndWhite="false" draft="false" cellComments="none" useFirstPageNumber="false" horizontalDpi="300" verticalDpi="300" copies="1"/>
+  <pageSetup paperSize="9" scale="100" firstPageNumber="0" fitToWidth="1" fitToHeight="1" pageOrder="downThenOver" orientation="portrait" usePrinterDefaults="false" blackAndWhite="false" draft="false" cellComments="none" useFirstPageNumber="false" horizontalDpi="300" verticalDpi="300" copies="1"/>
   <headerFooter differentFirst="false" differentOddEven="false">
     <oddHeader>&amp;C&amp;"Times New Roman,Regular"&amp;12&amp;A</oddHeader>
     <oddFooter>&amp;C&amp;"Times New Roman,Regular"&amp;12Page &amp;P</oddFooter>

</xml_diff>